<commit_message>
Added few more sensor's project list
</commit_message>
<xml_diff>
--- a/codelink.xlsx
+++ b/codelink.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="142">
   <si>
     <t>NO</t>
   </si>
@@ -361,6 +361,90 @@
   </si>
   <si>
     <t>5. Radiator Overheating Alarm in Cars</t>
+  </si>
+  <si>
+    <t>1. Plant Moisture Monitoring and Automation</t>
+  </si>
+  <si>
+    <t>2. Smart Irrigation System/Agriculture automation</t>
+  </si>
+  <si>
+    <t>3. To study Ground water recharge and Evapo-transpiration</t>
+  </si>
+  <si>
+    <t>1. Industrial and Home Security System</t>
+  </si>
+  <si>
+    <t>2. Challenge (bump) test for Sensor manufacturing companies</t>
+  </si>
+  <si>
+    <t>3. Fresh Air Monitoring / weather system</t>
+  </si>
+  <si>
+    <t>4. Leak Detaction in Factories</t>
+  </si>
+  <si>
+    <t>5. LPG leak detection in kitchen</t>
+  </si>
+  <si>
+    <t>1. Car wiper Automation</t>
+  </si>
+  <si>
+    <t>2. Smart drying Racks that automatically comes into house during rain</t>
+  </si>
+  <si>
+    <t>3. Home water Harvesting Automation</t>
+  </si>
+  <si>
+    <t>4. Check whether its raining or not in your mobile</t>
+  </si>
+  <si>
+    <t>5. Tweet for First Rain of the Season</t>
+  </si>
+  <si>
+    <t>1. Inside wearable device</t>
+  </si>
+  <si>
+    <t>2. In Hospital Automation</t>
+  </si>
+  <si>
+    <t>3. Traking heart-beat while daily workout ( in your mobile )</t>
+  </si>
+  <si>
+    <t>4. controls music with your heart beat</t>
+  </si>
+  <si>
+    <t>5. SMS alert to relative on High Heart Rate of Grand-father</t>
+  </si>
+  <si>
+    <t>1. Gesture controlled robot/car</t>
+  </si>
+  <si>
+    <t>2. Controlling 3D printed Human Hand</t>
+  </si>
+  <si>
+    <t>3. Virtual Reality Gaming Gloves</t>
+  </si>
+  <si>
+    <t>4. Knee Rehabitation Monitor</t>
+  </si>
+  <si>
+    <t>5. PPT/Presentation helping wearable</t>
+  </si>
+  <si>
+    <t>1. Alarm on full-filling water tank in house</t>
+  </si>
+  <si>
+    <t>2. Boiler water management/automation</t>
+  </si>
+  <si>
+    <t>3. Home Water Storage/Tank Monitoring &amp; Automation</t>
+  </si>
+  <si>
+    <t>4. River water level monitoring</t>
+  </si>
+  <si>
+    <t>5. Drinking Water Monitoring in Wedding Function</t>
   </si>
 </sst>
 </file>
@@ -709,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="C41" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -998,321 +1082,447 @@
       <c r="D32" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33">
+      <c r="E32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="E33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="E34" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
         <v>12</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>47</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>48</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D35" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="B34" t="s">
+      <c r="E35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="B36" t="s">
         <v>50</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>51</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D36" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35">
+      <c r="E36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="E37" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="E38" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="E39" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
         <v>13</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B40" t="s">
         <v>53</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C40" t="s">
         <v>54</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D40" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36">
+    <row r="41" spans="1:5">
+      <c r="A41">
         <v>14</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B41" t="s">
         <v>56</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C41" t="s">
         <v>57</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D41" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37">
+    <row r="42" spans="1:5">
+      <c r="A42">
         <v>15</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B42" t="s">
         <v>59</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C42" t="s">
         <v>60</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D42" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38">
+      <c r="E42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="E43" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="E44" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="E45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="E46" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
         <v>16</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B47" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39">
+      <c r="E47" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="E48" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="E49" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="E50" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="E51" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
         <v>17</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B52" t="s">
         <v>63</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C52" t="s">
         <v>64</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D52" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40">
+    <row r="53" spans="1:5">
+      <c r="A53">
         <v>18</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B53" t="s">
         <v>66</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C53" t="s">
         <v>67</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D53" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41">
+      <c r="E53" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="E54" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="E55" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="E56" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="E57" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
         <v>19</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B58" t="s">
         <v>69</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C58" t="s">
         <v>70</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D58" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42">
+    <row r="59" spans="1:5">
+      <c r="A59">
         <v>20</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B59" t="s">
         <v>72</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C59" t="s">
         <v>73</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D59" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43">
+      <c r="E59" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="E60" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="E61" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="E62" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="E63" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64">
         <v>21</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B64" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44">
+    <row r="65" spans="1:4">
+      <c r="A65">
         <v>22</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B65" t="s">
         <v>76</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C65" t="s">
         <v>77</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D65" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45">
+    <row r="66" spans="1:4">
+      <c r="A66">
         <v>23</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B66" t="s">
         <v>79</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C66" t="s">
         <v>80</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D66" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46">
+    <row r="67" spans="1:4">
+      <c r="A67">
         <v>24</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B67" t="s">
         <v>82</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C67" t="s">
         <v>83</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D67" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47">
+    <row r="68" spans="1:4">
+      <c r="A68">
         <v>25</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B68" t="s">
         <v>85</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C68" t="s">
         <v>86</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D68" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48">
+    <row r="69" spans="1:4">
+      <c r="A69">
         <v>26</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B69" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49">
+    <row r="70" spans="1:4">
+      <c r="A70">
         <v>27</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B70" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50">
+    <row r="71" spans="1:4">
+      <c r="A71">
         <v>28</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B71" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51">
+    <row r="72" spans="1:4">
+      <c r="A72">
         <v>29</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B72" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52">
+    <row r="73" spans="1:4">
+      <c r="A73">
         <v>30</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B73" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53">
+    <row r="74" spans="1:4">
+      <c r="A74">
         <v>31</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B74" t="s">
         <v>93</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C74" t="s">
         <v>94</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D74" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54">
+    <row r="75" spans="1:4">
+      <c r="A75">
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55">
+    <row r="76" spans="1:4">
+      <c r="A76">
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="1">
+    <row r="77" spans="1:4">
+      <c r="A77" s="1">
         <v>34</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B77" t="s">
         <v>96</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C77" t="s">
         <v>97</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D77" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="B57" t="s">
+    <row r="78" spans="1:4">
+      <c r="B78" t="s">
         <v>99</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C78" t="s">
         <v>100</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D78" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58">
+    <row r="79" spans="1:4">
+      <c r="A79">
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59">
+    <row r="80" spans="1:4">
+      <c r="A80">
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60">
+    <row r="81" spans="1:2">
+      <c r="A81">
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61">
+    <row r="82" spans="1:2">
+      <c r="A82">
         <v>38</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
-      <c r="A62">
+    <row r="83" spans="1:2">
+      <c r="A83">
         <v>39</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B83" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
-      <c r="A63">
+    <row r="84" spans="1:2">
+      <c r="A84">
         <v>40</v>
       </c>
     </row>

</xml_diff>